<commit_message>
Scaled the outrageous portfolio
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio - EBetancourt-TheOutrageousPortfolio EDITED.xlsx
+++ b/data/SJV Portfolio - EBetancourt-TheOutrageousPortfolio EDITED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6134EE9-0049-204D-ACC9-801640542F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE32D5E-EF93-BF4D-B11F-72C909812F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9C2185A5-4583-3441-AED7-AAC09E978B21}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="33900" windowHeight="17500" xr2:uid="{9C2185A5-4583-3441-AED7-AAC09E978B21}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio Design" sheetId="2" r:id="rId1"/>
@@ -422,7 +422,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -658,9 +658,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -698,7 +698,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -804,7 +804,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -946,7 +946,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -956,11 +956,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A6663F-1DBB-0040-A290-FFF68815F211}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="35.33203125" customWidth="1"/>
@@ -969,13 +969,13 @@
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="44" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="115" customHeight="1">
+    <row r="2" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
@@ -987,7 +987,7 @@
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
     </row>
-    <row r="3" spans="1:6" ht="31">
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1001,7 +1001,7 @@
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -1011,7 +1011,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="21"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -1021,7 +1021,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -1031,7 +1031,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -1041,7 +1041,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
@@ -1051,7 +1051,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="14" customHeight="1">
+    <row r="9" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1061,26 +1061,26 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D10" s="23" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D11" s="23" t="s">
         <v>57</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" s="6" customFormat="1">
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="7" customFormat="1">
+    <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>4</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="10">
-        <v>3</v>
+        <v>5.7692307692307692</v>
       </c>
       <c r="D28" s="11">
         <v>3</v>
@@ -1404,7 +1404,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="10">
-        <v>3</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="D29" s="11">
         <v>3</v>
@@ -1424,7 +1424,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1504,14 +1504,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>40</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
         <v>44</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>45</v>
       </c>
@@ -1565,17 +1565,17 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" customWidth="1"/>
     <col min="2" max="2" width="37.5" customWidth="1"/>
     <col min="6" max="25" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>117000</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>310000</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>99500</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>99500</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2885,90 +2885,90 @@
       </c>
       <c r="F14" s="25">
         <f t="shared" si="1"/>
-        <v>142.85714285714286</v>
+        <v>274.72527472527474</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>285.71428571428572</v>
+        <v>549.45054945054949</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>428.57142857142856</v>
+        <v>824.17582417582423</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>571.42857142857144</v>
+        <v>1098.901098901099</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>714.28571428571433</v>
+        <v>1373.6263736263736</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>857.14285714285722</v>
+        <v>1648.3516483516482</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>1000.0000000000001</v>
+        <v>1923.0769230769229</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>1142.8571428571429</v>
+        <v>2197.8021978021975</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>1285.7142857142858</v>
+        <v>2472.5274725274721</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>1428.5714285714287</v>
+        <v>2747.2527472527468</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>1571.4285714285716</v>
+        <v>3021.9780219780214</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>1714.2857142857144</v>
+        <v>3296.703296703296</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>1857.1428571428573</v>
+        <v>3571.4285714285706</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>2000.0000000000002</v>
+        <v>3846.1538461538453</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>2142.8571428571431</v>
+        <v>4120.8791208791199</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>2285.7142857142858</v>
+        <v>4395.604395604395</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>2428.5714285714284</v>
+        <v>4670.3296703296701</v>
       </c>
       <c r="W14">
         <f t="shared" si="0"/>
-        <v>2571.4285714285711</v>
+        <v>4945.0549450549452</v>
       </c>
       <c r="X14">
         <f t="shared" si="0"/>
-        <v>2714.2857142857138</v>
+        <v>5219.7802197802202</v>
       </c>
       <c r="Y14">
         <f t="shared" si="0"/>
-        <v>2857.1428571428564</v>
+        <v>5494.5054945054953</v>
       </c>
       <c r="Z14" s="25">
         <f>'Portfolio Design'!C28*1000</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
+        <v>5769.2307692307695</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2986,90 +2986,90 @@
       </c>
       <c r="F15" s="25">
         <f t="shared" si="1"/>
+        <v>10.989010989010989</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>21.978021978021978</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>32.967032967032964</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>43.956043956043956</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>54.945054945054949</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>65.934065934065941</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>76.923076923076934</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>87.912087912087927</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>98.901098901098919</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>109.89010989010991</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="2"/>
+        <v>120.8791208791209</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="2"/>
+        <v>131.86813186813188</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="2"/>
         <v>142.85714285714286</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="2"/>
-        <v>285.71428571428572</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>428.57142857142856</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
-        <v>571.42857142857144</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
-        <v>714.28571428571433</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="2"/>
-        <v>857.14285714285722</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>1000.0000000000001</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>1142.8571428571429</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="2"/>
-        <v>1285.7142857142858</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="2"/>
-        <v>1428.5714285714287</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="2"/>
-        <v>1571.4285714285716</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="2"/>
-        <v>1714.2857142857144</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="2"/>
-        <v>1857.1428571428573</v>
-      </c>
       <c r="S15">
         <f t="shared" si="2"/>
-        <v>2000.0000000000002</v>
+        <v>153.84615384615384</v>
       </c>
       <c r="T15">
         <f t="shared" si="2"/>
-        <v>2142.8571428571431</v>
+        <v>164.83516483516482</v>
       </c>
       <c r="U15">
         <f t="shared" si="2"/>
-        <v>2285.7142857142858</v>
+        <v>175.8241758241758</v>
       </c>
       <c r="V15">
         <f t="shared" si="2"/>
-        <v>2428.5714285714284</v>
+        <v>186.81318681318677</v>
       </c>
       <c r="W15">
         <f t="shared" si="0"/>
-        <v>2571.4285714285711</v>
+        <v>197.80219780219775</v>
       </c>
       <c r="X15">
         <f t="shared" si="0"/>
-        <v>2714.2857142857138</v>
+        <v>208.79120879120873</v>
       </c>
       <c r="Y15">
         <f t="shared" si="0"/>
-        <v>2857.1428571428564</v>
+        <v>219.78021978021971</v>
       </c>
       <c r="Z15" s="25">
         <f>'Portfolio Design'!C29*1000</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
+        <v>230.76923076923077</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -3385,13 +3385,13 @@
       <selection activeCell="C3" sqref="C3:W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>69</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>10</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>24</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>33</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3993,9 +3993,9 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>

</xml_diff>